<commit_message>
we e e e
</commit_message>
<xml_diff>
--- a/The research project/LCDMA_February_2023/Table_can_md.xlsx
+++ b/The research project/LCDMA_February_2023/Table_can_md.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo9\Dropbox\CAN_MD\LCDMA_February_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tie/Documents/GitHub/ECON-493-forcasting-economy/The research project/LCDMA_February_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AB35E2-1F3D-4A68-872D-7BB90187A864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7621F0DB-B081-4A42-8E10-59DA5BEDB373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B44822A1-C94B-47DB-A854-B820FCC2AF64}"/>
+    <workbookView xWindow="25120" yWindow="4560" windowWidth="29040" windowHeight="15840" xr2:uid="{B44822A1-C94B-47DB-A854-B820FCC2AF64}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3401,18 +3401,19 @@
     <t>v1230996001</t>
   </si>
   <si>
-    <t xml:space="preserve">v122530	</t>
+    <t>New housing price index, Total (house and land)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3426,7 +3427,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3483,7 +3484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3499,7 +3500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3797,19 +3798,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8B8EAC-8362-4A6B-85ED-20AE75E9042C}">
   <dimension ref="A1:H453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>356</v>
       </c>
@@ -3835,7 +3836,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4069,7 +4070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4173,7 +4174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4199,7 +4200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4279,7 +4280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4299,7 +4300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4339,7 +4340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4359,7 +4360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4385,7 +4386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4425,7 +4426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4445,7 +4446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4465,7 +4466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4531,7 +4532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4579,7 +4580,7 @@
         <v>1005</v>
       </c>
       <c r="C34" t="s">
-        <v>993</v>
+        <v>1122</v>
       </c>
       <c r="D34" t="s">
         <v>364</v>
@@ -4591,7 +4592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4651,7 +4652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4731,7 +4732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4817,7 +4818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4843,7 +4844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4869,7 +4870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4921,7 +4922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4947,7 +4948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5025,7 +5026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5077,7 +5078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5129,7 +5130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5181,7 +5182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5207,7 +5208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5233,7 +5234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5259,7 +5260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5285,7 +5286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5337,7 +5338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5363,7 +5364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5389,7 +5390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5415,7 +5416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5441,7 +5442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5493,7 +5494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5519,7 +5520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5571,7 +5572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5597,7 +5598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5623,7 +5624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5649,7 +5650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5675,7 +5676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5727,7 +5728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5753,7 +5754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5779,7 +5780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5831,7 +5832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5857,7 +5858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5883,7 +5884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5935,7 +5936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5961,7 +5962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6013,7 +6014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6039,7 +6040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6065,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6091,7 +6092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6117,7 +6118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6143,7 +6144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6169,7 +6170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6189,7 +6190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6209,7 +6210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6229,7 +6230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6249,7 +6250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6269,7 +6270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6309,7 +6310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6329,7 +6330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6349,7 +6350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6403,13 +6404,13 @@
         <v>364</v>
       </c>
       <c r="E109" t="s">
-        <v>1122</v>
+        <v>1106</v>
       </c>
       <c r="H109">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6429,7 +6430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6449,7 +6450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6469,7 +6470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6489,7 +6490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6515,7 +6516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115">
         <v>114</v>
       </c>
@@ -6541,7 +6542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117">
         <v>116</v>
       </c>
@@ -6581,7 +6582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6601,7 +6602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6661,7 +6662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6681,7 +6682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123">
         <v>122</v>
       </c>
@@ -6701,7 +6702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124">
         <v>123</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125">
         <v>124</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126">
         <v>125</v>
       </c>
@@ -6767,7 +6768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="A127">
         <v>126</v>
       </c>
@@ -6793,7 +6794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128">
         <v>127</v>
       </c>
@@ -6819,7 +6820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6845,7 +6846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="B131" t="s">
         <v>710</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="B132" t="s">
         <v>710</v>
       </c>
@@ -6911,7 +6912,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="B133" t="s">
         <v>710</v>
       </c>
@@ -6931,7 +6932,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134">
         <v>130</v>
       </c>
@@ -6957,7 +6958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="B135" t="s">
         <v>710</v>
       </c>
@@ -6977,7 +6978,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="B136" t="s">
         <v>710</v>
       </c>
@@ -6997,7 +6998,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="B137" t="s">
         <v>710</v>
       </c>
@@ -7017,7 +7018,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="B138" t="s">
         <v>710</v>
       </c>
@@ -7037,7 +7038,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="B139" t="s">
         <v>710</v>
       </c>
@@ -7057,7 +7058,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140">
         <v>131</v>
       </c>
@@ -7083,7 +7084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="B141" t="s">
         <v>710</v>
       </c>
@@ -7103,7 +7104,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="B142" t="s">
         <v>710</v>
       </c>
@@ -7123,7 +7124,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="B143" t="s">
         <v>710</v>
       </c>
@@ -7143,7 +7144,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="B144" t="s">
         <v>710</v>
       </c>
@@ -7163,7 +7164,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="B145" t="s">
         <v>710</v>
       </c>
@@ -7183,7 +7184,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="B146" t="s">
         <v>710</v>
       </c>
@@ -7203,7 +7204,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="B147" t="s">
         <v>710</v>
       </c>
@@ -7223,7 +7224,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="B148" t="s">
         <v>710</v>
       </c>
@@ -7243,7 +7244,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="B149" t="s">
         <v>710</v>
       </c>
@@ -7263,7 +7264,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="B150" t="s">
         <v>710</v>
       </c>
@@ -7283,7 +7284,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151">
         <v>132</v>
       </c>
@@ -7309,7 +7310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="B152" t="s">
         <v>710</v>
       </c>
@@ -7329,7 +7330,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="B153" t="s">
         <v>710</v>
       </c>
@@ -7349,7 +7350,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8">
       <c r="A154">
         <v>133</v>
       </c>
@@ -7375,7 +7376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="B155" t="s">
         <v>710</v>
       </c>
@@ -7395,7 +7396,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8">
       <c r="B156" t="s">
         <v>710</v>
       </c>
@@ -7415,7 +7416,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8">
       <c r="A157">
         <v>134</v>
       </c>
@@ -7441,7 +7442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8">
       <c r="B158" t="s">
         <v>710</v>
       </c>
@@ -7461,7 +7462,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8">
       <c r="B159" t="s">
         <v>710</v>
       </c>
@@ -7481,7 +7482,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8">
       <c r="A160">
         <v>135</v>
       </c>
@@ -7507,7 +7508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="B161" t="s">
         <v>710</v>
       </c>
@@ -7527,7 +7528,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8">
       <c r="B162" t="s">
         <v>710</v>
       </c>
@@ -7547,7 +7548,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8">
       <c r="B163" t="s">
         <v>710</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="B164" t="s">
         <v>710</v>
       </c>
@@ -7587,7 +7588,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="B165" t="s">
         <v>710</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8">
       <c r="A166">
         <v>136</v>
       </c>
@@ -7633,7 +7634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8">
       <c r="B167" t="s">
         <v>710</v>
       </c>
@@ -7653,7 +7654,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8">
       <c r="B168" t="s">
         <v>710</v>
       </c>
@@ -7673,7 +7674,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8">
       <c r="B169" t="s">
         <v>710</v>
       </c>
@@ -7693,7 +7694,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8">
       <c r="B170" t="s">
         <v>710</v>
       </c>
@@ -7713,7 +7714,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8">
       <c r="B171" t="s">
         <v>710</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8">
       <c r="A172">
         <v>137</v>
       </c>
@@ -7759,7 +7760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8">
       <c r="B173" t="s">
         <v>710</v>
       </c>
@@ -7779,7 +7780,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8">
       <c r="B174" t="s">
         <v>710</v>
       </c>
@@ -7799,7 +7800,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8">
       <c r="A175">
         <v>138</v>
       </c>
@@ -7825,7 +7826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8">
       <c r="B176" t="s">
         <v>710</v>
       </c>
@@ -7845,7 +7846,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8">
       <c r="B177" t="s">
         <v>710</v>
       </c>
@@ -7865,7 +7866,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8">
       <c r="B178" t="s">
         <v>710</v>
       </c>
@@ -7885,7 +7886,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8">
       <c r="B179" t="s">
         <v>710</v>
       </c>
@@ -7905,7 +7906,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8">
       <c r="B180" t="s">
         <v>710</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8">
       <c r="A181">
         <v>139</v>
       </c>
@@ -7951,7 +7952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8">
       <c r="A182">
         <v>140</v>
       </c>
@@ -7977,7 +7978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8">
       <c r="A183">
         <v>141</v>
       </c>
@@ -8003,7 +8004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8">
       <c r="A184">
         <v>142</v>
       </c>
@@ -8023,7 +8024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8">
       <c r="A185">
         <v>143</v>
       </c>
@@ -8043,7 +8044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8">
       <c r="A186">
         <v>144</v>
       </c>
@@ -8063,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8">
       <c r="A187">
         <v>145</v>
       </c>
@@ -8083,7 +8084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8">
       <c r="A188">
         <v>146</v>
       </c>
@@ -8103,7 +8104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8">
       <c r="A189">
         <v>147</v>
       </c>
@@ -8123,7 +8124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8">
       <c r="A190">
         <v>148</v>
       </c>
@@ -8143,7 +8144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8">
       <c r="A191">
         <v>149</v>
       </c>
@@ -8163,7 +8164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8">
       <c r="A192">
         <v>150</v>
       </c>
@@ -8183,7 +8184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8">
       <c r="A193">
         <v>151</v>
       </c>
@@ -8203,7 +8204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8">
       <c r="A194">
         <v>152</v>
       </c>
@@ -8223,7 +8224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8">
       <c r="A195">
         <v>153</v>
       </c>
@@ -8243,7 +8244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8">
       <c r="A196">
         <v>154</v>
       </c>
@@ -8263,7 +8264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8">
       <c r="A197">
         <v>155</v>
       </c>
@@ -8283,7 +8284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8">
       <c r="A198">
         <v>156</v>
       </c>
@@ -8303,7 +8304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8">
       <c r="A199">
         <v>157</v>
       </c>
@@ -8323,7 +8324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8">
       <c r="A200">
         <v>158</v>
       </c>
@@ -8343,7 +8344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8">
       <c r="A201">
         <v>159</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8">
       <c r="A202">
         <v>160</v>
       </c>
@@ -8383,7 +8384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8">
       <c r="A203">
         <v>161</v>
       </c>
@@ -8400,7 +8401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8">
       <c r="A204">
         <v>162</v>
       </c>
@@ -8417,7 +8418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8">
       <c r="A205">
         <v>163</v>
       </c>
@@ -8434,7 +8435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8">
       <c r="A206">
         <v>164</v>
       </c>
@@ -8451,7 +8452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8">
       <c r="A207">
         <v>165</v>
       </c>
@@ -8477,7 +8478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8">
       <c r="A208">
         <v>166</v>
       </c>
@@ -8497,7 +8498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8">
       <c r="A209">
         <v>167</v>
       </c>
@@ -8517,7 +8518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8">
       <c r="A210">
         <v>168</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8">
       <c r="A211">
         <v>169</v>
       </c>
@@ -8557,7 +8558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8">
       <c r="A212">
         <v>170</v>
       </c>
@@ -8577,7 +8578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8">
       <c r="A213">
         <v>171</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8">
       <c r="A214">
         <v>172</v>
       </c>
@@ -8617,7 +8618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8">
       <c r="A215">
         <v>173</v>
       </c>
@@ -8637,7 +8638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8">
       <c r="A216">
         <v>174</v>
       </c>
@@ -8657,7 +8658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8">
       <c r="A217">
         <v>175</v>
       </c>
@@ -8677,7 +8678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8">
       <c r="A218">
         <v>176</v>
       </c>
@@ -8697,7 +8698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8">
       <c r="A219">
         <v>177</v>
       </c>
@@ -8717,7 +8718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8">
       <c r="A220">
         <v>178</v>
       </c>
@@ -8737,7 +8738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8">
       <c r="A221">
         <v>179</v>
       </c>
@@ -8757,7 +8758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8">
       <c r="A222">
         <v>180</v>
       </c>
@@ -8777,7 +8778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8">
       <c r="A223">
         <v>181</v>
       </c>
@@ -8797,7 +8798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8">
       <c r="A224">
         <v>182</v>
       </c>
@@ -8817,7 +8818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8">
       <c r="A225">
         <v>183</v>
       </c>
@@ -8837,7 +8838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8">
       <c r="A226">
         <v>184</v>
       </c>
@@ -8857,7 +8858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8">
       <c r="A227">
         <v>185</v>
       </c>
@@ -8877,7 +8878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8">
       <c r="A228">
         <v>186</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8">
       <c r="A229">
         <v>187</v>
       </c>
@@ -8917,7 +8918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8">
       <c r="A230">
         <v>188</v>
       </c>
@@ -8937,7 +8938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8">
       <c r="A231">
         <v>189</v>
       </c>
@@ -8957,7 +8958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8">
       <c r="A232">
         <v>190</v>
       </c>
@@ -8977,7 +8978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8">
       <c r="A233">
         <v>191</v>
       </c>
@@ -8997,7 +8998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8">
       <c r="A234">
         <v>192</v>
       </c>
@@ -9017,7 +9018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8">
       <c r="A235">
         <v>193</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8">
       <c r="A236">
         <v>194</v>
       </c>
@@ -9057,7 +9058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8">
       <c r="A237">
         <v>195</v>
       </c>
@@ -9077,7 +9078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8">
       <c r="A238">
         <v>196</v>
       </c>
@@ -9097,7 +9098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8">
       <c r="A239">
         <v>197</v>
       </c>
@@ -9117,7 +9118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8">
       <c r="A240">
         <v>198</v>
       </c>
@@ -9137,7 +9138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8">
       <c r="A241">
         <v>199</v>
       </c>
@@ -9157,7 +9158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8">
       <c r="A242">
         <v>200</v>
       </c>
@@ -9177,7 +9178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8">
       <c r="A243">
         <v>201</v>
       </c>
@@ -9197,7 +9198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8">
       <c r="A244">
         <v>202</v>
       </c>
@@ -9217,7 +9218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8">
       <c r="A245">
         <v>203</v>
       </c>
@@ -9237,7 +9238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8">
       <c r="A246">
         <v>204</v>
       </c>
@@ -9257,7 +9258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8">
       <c r="A247">
         <v>205</v>
       </c>
@@ -9277,7 +9278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8">
       <c r="A248">
         <v>206</v>
       </c>
@@ -9297,7 +9298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8">
       <c r="A249">
         <v>207</v>
       </c>
@@ -9317,7 +9318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8">
       <c r="A250">
         <v>208</v>
       </c>
@@ -9337,7 +9338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8">
       <c r="A251">
         <v>209</v>
       </c>
@@ -9357,7 +9358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8">
       <c r="A252">
         <v>210</v>
       </c>
@@ -9377,7 +9378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8">
       <c r="A253">
         <v>211</v>
       </c>
@@ -9397,7 +9398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8">
       <c r="A254">
         <v>212</v>
       </c>
@@ -9417,7 +9418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8">
       <c r="A255">
         <v>213</v>
       </c>
@@ -9437,7 +9438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8">
       <c r="A256">
         <v>214</v>
       </c>
@@ -9457,7 +9458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8">
       <c r="A257">
         <v>215</v>
       </c>
@@ -9477,7 +9478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8">
       <c r="A258">
         <v>216</v>
       </c>
@@ -9497,7 +9498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8">
       <c r="A259">
         <v>217</v>
       </c>
@@ -9517,7 +9518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8">
       <c r="A260">
         <v>218</v>
       </c>
@@ -9537,7 +9538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8">
       <c r="A261">
         <v>219</v>
       </c>
@@ -9557,7 +9558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8">
       <c r="A262">
         <v>220</v>
       </c>
@@ -9577,7 +9578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8">
       <c r="A263">
         <v>221</v>
       </c>
@@ -9597,7 +9598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8">
       <c r="A264">
         <v>222</v>
       </c>
@@ -9617,7 +9618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8">
       <c r="A265">
         <v>223</v>
       </c>
@@ -9637,7 +9638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8">
       <c r="A266">
         <v>224</v>
       </c>
@@ -9657,7 +9658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8">
       <c r="A267">
         <v>225</v>
       </c>
@@ -9677,7 +9678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8">
       <c r="A268">
         <v>226</v>
       </c>
@@ -9697,7 +9698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8">
       <c r="A269">
         <v>227</v>
       </c>
@@ -9717,7 +9718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8">
       <c r="A270">
         <v>228</v>
       </c>
@@ -9737,7 +9738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8">
       <c r="A271">
         <v>229</v>
       </c>
@@ -9757,7 +9758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8">
       <c r="A272">
         <v>230</v>
       </c>
@@ -9777,7 +9778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8">
       <c r="A273">
         <v>231</v>
       </c>
@@ -9797,7 +9798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8">
       <c r="A274">
         <v>232</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8">
       <c r="A275">
         <v>233</v>
       </c>
@@ -9837,7 +9838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8">
       <c r="A276">
         <v>234</v>
       </c>
@@ -9857,7 +9858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8">
       <c r="A277">
         <v>235</v>
       </c>
@@ -9877,7 +9878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8">
       <c r="A278">
         <v>236</v>
       </c>
@@ -9897,7 +9898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8">
       <c r="A279">
         <v>237</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8">
       <c r="A280">
         <v>238</v>
       </c>
@@ -9937,7 +9938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8">
       <c r="A281">
         <v>239</v>
       </c>
@@ -9957,7 +9958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8">
       <c r="A282">
         <v>240</v>
       </c>
@@ -9977,7 +9978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8">
       <c r="A283">
         <v>241</v>
       </c>
@@ -9997,7 +9998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8">
       <c r="A284">
         <v>242</v>
       </c>
@@ -10017,7 +10018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8">
       <c r="A285">
         <v>243</v>
       </c>
@@ -10037,7 +10038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8">
       <c r="A286">
         <v>244</v>
       </c>
@@ -10057,7 +10058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8">
       <c r="A287">
         <v>245</v>
       </c>
@@ -10077,7 +10078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8">
       <c r="A288">
         <v>246</v>
       </c>
@@ -10097,7 +10098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8">
       <c r="A289">
         <v>247</v>
       </c>
@@ -10117,7 +10118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8">
       <c r="A290">
         <v>248</v>
       </c>
@@ -10137,7 +10138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8">
       <c r="A291">
         <v>249</v>
       </c>
@@ -10157,7 +10158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8">
       <c r="A292">
         <v>250</v>
       </c>
@@ -10177,7 +10178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8">
       <c r="A293">
         <v>251</v>
       </c>
@@ -10197,7 +10198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8">
       <c r="A294">
         <v>252</v>
       </c>
@@ -10217,7 +10218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8">
       <c r="A295">
         <v>253</v>
       </c>
@@ -10237,7 +10238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8">
       <c r="A296">
         <v>254</v>
       </c>
@@ -10257,7 +10258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8">
       <c r="A297">
         <v>255</v>
       </c>
@@ -10277,7 +10278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8">
       <c r="A298">
         <v>256</v>
       </c>
@@ -10300,7 +10301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8">
       <c r="A299">
         <v>257</v>
       </c>
@@ -10323,7 +10324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8">
       <c r="A300">
         <v>258</v>
       </c>
@@ -10346,7 +10347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8">
       <c r="A301">
         <v>259</v>
       </c>
@@ -10369,7 +10370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8">
       <c r="A302">
         <v>260</v>
       </c>
@@ -10392,7 +10393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8">
       <c r="A303">
         <v>261</v>
       </c>
@@ -10415,7 +10416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8">
       <c r="A304">
         <v>262</v>
       </c>
@@ -10438,7 +10439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8">
       <c r="A305">
         <v>263</v>
       </c>
@@ -10461,7 +10462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8">
       <c r="A306">
         <v>264</v>
       </c>
@@ -10484,7 +10485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8">
       <c r="A307">
         <v>265</v>
       </c>
@@ -10507,7 +10508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8">
       <c r="A308">
         <v>266</v>
       </c>
@@ -10527,7 +10528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8">
       <c r="A309">
         <v>267</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8">
       <c r="A310">
         <v>268</v>
       </c>
@@ -10567,7 +10568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8">
       <c r="A311">
         <v>269</v>
       </c>
@@ -10587,7 +10588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8">
       <c r="A312">
         <v>270</v>
       </c>
@@ -10607,7 +10608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8">
       <c r="A313">
         <v>271</v>
       </c>
@@ -10627,7 +10628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8">
       <c r="A314">
         <v>272</v>
       </c>
@@ -10647,7 +10648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8">
       <c r="A315">
         <v>273</v>
       </c>
@@ -10667,7 +10668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8">
       <c r="A316">
         <v>274</v>
       </c>
@@ -10687,7 +10688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8">
       <c r="A317">
         <v>275</v>
       </c>
@@ -10707,7 +10708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8">
       <c r="A318">
         <v>276</v>
       </c>
@@ -10727,7 +10728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8">
       <c r="A319">
         <v>277</v>
       </c>
@@ -10747,7 +10748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8">
       <c r="A320">
         <v>278</v>
       </c>
@@ -10767,7 +10768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8">
       <c r="A321">
         <v>279</v>
       </c>
@@ -10787,7 +10788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8">
       <c r="A322">
         <v>280</v>
       </c>
@@ -10807,7 +10808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8">
       <c r="A323">
         <v>281</v>
       </c>
@@ -10827,7 +10828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8">
       <c r="A324">
         <v>282</v>
       </c>
@@ -10847,7 +10848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8">
       <c r="A325">
         <v>283</v>
       </c>
@@ -10867,7 +10868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8">
       <c r="A326">
         <v>284</v>
       </c>
@@ -10887,7 +10888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8">
       <c r="A327">
         <v>285</v>
       </c>
@@ -10907,7 +10908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8">
       <c r="A328">
         <v>286</v>
       </c>
@@ -10927,7 +10928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8">
       <c r="A329">
         <v>287</v>
       </c>
@@ -10947,7 +10948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8">
       <c r="A330">
         <v>288</v>
       </c>
@@ -10967,7 +10968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8">
       <c r="A331">
         <v>289</v>
       </c>
@@ -10987,7 +10988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8">
       <c r="A332">
         <v>290</v>
       </c>
@@ -11007,7 +11008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8">
       <c r="A333">
         <v>291</v>
       </c>
@@ -11027,7 +11028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8">
       <c r="A334">
         <v>292</v>
       </c>
@@ -11047,7 +11048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8">
       <c r="A335">
         <v>293</v>
       </c>
@@ -11067,7 +11068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8">
       <c r="A336">
         <v>294</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8">
       <c r="A337">
         <v>295</v>
       </c>
@@ -11107,7 +11108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8">
       <c r="A338">
         <v>296</v>
       </c>
@@ -11133,7 +11134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8">
       <c r="A339">
         <v>297</v>
       </c>
@@ -11159,7 +11160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8">
       <c r="A340">
         <v>298</v>
       </c>
@@ -11185,7 +11186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8">
       <c r="A341">
         <v>299</v>
       </c>
@@ -11211,7 +11212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8">
       <c r="A342">
         <v>300</v>
       </c>
@@ -11237,7 +11238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8">
       <c r="A343">
         <v>301</v>
       </c>
@@ -11263,7 +11264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8">
       <c r="A344">
         <v>302</v>
       </c>
@@ -11289,7 +11290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8">
       <c r="A345">
         <v>303</v>
       </c>
@@ -11315,7 +11316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8">
       <c r="A346">
         <v>304</v>
       </c>
@@ -11341,7 +11342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8">
       <c r="A347">
         <v>305</v>
       </c>
@@ -11367,7 +11368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8">
       <c r="A348">
         <v>306</v>
       </c>
@@ -11393,7 +11394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8">
       <c r="A349">
         <v>307</v>
       </c>
@@ -11419,7 +11420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8">
       <c r="A350">
         <v>308</v>
       </c>
@@ -11445,7 +11446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8">
       <c r="A351">
         <v>309</v>
       </c>
@@ -11471,7 +11472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8">
       <c r="A352">
         <v>310</v>
       </c>
@@ -11497,7 +11498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8">
       <c r="A353">
         <v>311</v>
       </c>
@@ -11523,7 +11524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8">
       <c r="A354">
         <v>312</v>
       </c>
@@ -11549,7 +11550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8">
       <c r="A355">
         <v>313</v>
       </c>
@@ -11575,7 +11576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8">
       <c r="A356">
         <v>314</v>
       </c>
@@ -11601,7 +11602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8">
       <c r="A357">
         <v>315</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8">
       <c r="A358">
         <v>316</v>
       </c>
@@ -11647,7 +11648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8">
       <c r="A359">
         <v>317</v>
       </c>
@@ -11667,7 +11668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8">
       <c r="A360">
         <v>318</v>
       </c>
@@ -11687,7 +11688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8">
       <c r="A361">
         <v>319</v>
       </c>
@@ -11707,7 +11708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8">
       <c r="A362">
         <v>320</v>
       </c>
@@ -11727,7 +11728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8">
       <c r="A363">
         <v>321</v>
       </c>
@@ -11747,7 +11748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8">
       <c r="A364">
         <v>322</v>
       </c>
@@ -11767,7 +11768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8">
       <c r="A365">
         <v>323</v>
       </c>
@@ -11787,7 +11788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8">
       <c r="A366">
         <v>324</v>
       </c>
@@ -11807,7 +11808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8">
       <c r="A367">
         <v>325</v>
       </c>
@@ -11827,7 +11828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8">
       <c r="A368">
         <v>326</v>
       </c>
@@ -11847,7 +11848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8">
       <c r="A369">
         <v>327</v>
       </c>
@@ -11867,7 +11868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8">
       <c r="A370">
         <v>328</v>
       </c>
@@ -11887,7 +11888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8">
       <c r="A371">
         <v>329</v>
       </c>
@@ -11907,7 +11908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8">
       <c r="A372">
         <v>330</v>
       </c>
@@ -11927,7 +11928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8">
       <c r="A373">
         <v>331</v>
       </c>
@@ -11947,7 +11948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8">
       <c r="A374">
         <v>332</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8">
       <c r="A375">
         <v>333</v>
       </c>
@@ -11987,7 +11988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8">
       <c r="A376">
         <v>334</v>
       </c>
@@ -12007,7 +12008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8">
       <c r="A377">
         <v>335</v>
       </c>
@@ -12027,7 +12028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8">
       <c r="A378">
         <v>336</v>
       </c>
@@ -12047,7 +12048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8">
       <c r="A379">
         <v>337</v>
       </c>
@@ -12067,7 +12068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8">
       <c r="A380">
         <v>338</v>
       </c>
@@ -12087,7 +12088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8">
       <c r="A381">
         <v>339</v>
       </c>
@@ -12107,7 +12108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8">
       <c r="A382">
         <v>340</v>
       </c>
@@ -12127,7 +12128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8">
       <c r="A383">
         <v>341</v>
       </c>
@@ -12147,7 +12148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8">
       <c r="A384">
         <v>342</v>
       </c>
@@ -12167,7 +12168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8">
       <c r="A385">
         <v>343</v>
       </c>
@@ -12187,7 +12188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8">
       <c r="A386">
         <v>344</v>
       </c>
@@ -12207,7 +12208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8">
       <c r="A387">
         <v>345</v>
       </c>
@@ -12227,7 +12228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8">
       <c r="A388">
         <v>346</v>
       </c>
@@ -12247,7 +12248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8">
       <c r="A389">
         <v>347</v>
       </c>
@@ -12267,7 +12268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8">
       <c r="A390">
         <v>348</v>
       </c>
@@ -12287,7 +12288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8">
       <c r="A391">
         <v>349</v>
       </c>
@@ -12307,7 +12308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8">
       <c r="A392">
         <v>350</v>
       </c>
@@ -12327,7 +12328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8">
       <c r="A393">
         <v>351</v>
       </c>
@@ -12347,7 +12348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8">
       <c r="A394">
         <v>352</v>
       </c>
@@ -12367,7 +12368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8">
       <c r="A395">
         <v>353</v>
       </c>
@@ -12387,7 +12388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8">
       <c r="A396">
         <v>354</v>
       </c>
@@ -12407,7 +12408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8">
       <c r="A397">
         <v>355</v>
       </c>
@@ -12427,7 +12428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8">
       <c r="A398">
         <v>356</v>
       </c>
@@ -12447,7 +12448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8">
       <c r="A399">
         <v>357</v>
       </c>
@@ -12467,7 +12468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8">
       <c r="A400">
         <v>358</v>
       </c>
@@ -12487,7 +12488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8">
       <c r="A401">
         <v>359</v>
       </c>
@@ -12507,7 +12508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8">
       <c r="A402">
         <v>360</v>
       </c>
@@ -12527,7 +12528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8">
       <c r="A403">
         <v>361</v>
       </c>
@@ -12547,7 +12548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8">
       <c r="A404">
         <v>362</v>
       </c>
@@ -12567,7 +12568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8">
       <c r="A405">
         <v>363</v>
       </c>
@@ -12587,7 +12588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8">
       <c r="A406">
         <v>364</v>
       </c>
@@ -12607,7 +12608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8">
       <c r="A407">
         <v>365</v>
       </c>
@@ -12627,7 +12628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8">
       <c r="A408">
         <v>366</v>
       </c>
@@ -12647,7 +12648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8">
       <c r="A409">
         <v>367</v>
       </c>
@@ -12667,7 +12668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8">
       <c r="A410">
         <v>368</v>
       </c>
@@ -12687,7 +12688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8">
       <c r="A411">
         <v>369</v>
       </c>
@@ -12707,7 +12708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8">
       <c r="A412">
         <v>370</v>
       </c>
@@ -12727,7 +12728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8">
       <c r="A413">
         <v>371</v>
       </c>
@@ -12747,7 +12748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8">
       <c r="A414">
         <v>372</v>
       </c>
@@ -12767,7 +12768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8">
       <c r="A415">
         <v>373</v>
       </c>
@@ -12787,7 +12788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8">
       <c r="A416">
         <v>374</v>
       </c>
@@ -12807,7 +12808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8">
       <c r="A417">
         <v>375</v>
       </c>
@@ -12827,7 +12828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8">
       <c r="A418">
         <v>376</v>
       </c>
@@ -12847,7 +12848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8">
       <c r="A419">
         <v>377</v>
       </c>
@@ -12867,7 +12868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8">
       <c r="A420">
         <v>378</v>
       </c>
@@ -12887,7 +12888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8">
       <c r="A421">
         <v>379</v>
       </c>
@@ -12907,7 +12908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8">
       <c r="A422">
         <v>380</v>
       </c>
@@ -12927,7 +12928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8">
       <c r="A423">
         <v>381</v>
       </c>
@@ -12947,7 +12948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8">
       <c r="A424">
         <v>382</v>
       </c>
@@ -12967,7 +12968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8">
       <c r="A425">
         <v>383</v>
       </c>
@@ -12987,7 +12988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8">
       <c r="A426">
         <v>384</v>
       </c>
@@ -13007,7 +13008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8">
       <c r="A427">
         <v>385</v>
       </c>
@@ -13027,7 +13028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8">
       <c r="A428">
         <v>386</v>
       </c>
@@ -13047,7 +13048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8">
       <c r="A429">
         <v>387</v>
       </c>
@@ -13067,7 +13068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8">
       <c r="A430">
         <v>388</v>
       </c>
@@ -13087,7 +13088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8">
       <c r="A431">
         <v>389</v>
       </c>
@@ -13107,7 +13108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8">
       <c r="A432">
         <v>390</v>
       </c>
@@ -13127,7 +13128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8">
       <c r="A433">
         <v>391</v>
       </c>
@@ -13147,7 +13148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8">
       <c r="A434">
         <v>392</v>
       </c>
@@ -13167,7 +13168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8">
       <c r="A435">
         <v>393</v>
       </c>
@@ -13187,7 +13188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8">
       <c r="A436">
         <v>394</v>
       </c>
@@ -13207,7 +13208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8">
       <c r="A437">
         <v>395</v>
       </c>
@@ -13227,7 +13228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8">
       <c r="A438">
         <v>396</v>
       </c>
@@ -13247,7 +13248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8">
       <c r="A439">
         <v>397</v>
       </c>
@@ -13267,7 +13268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8">
       <c r="A440">
         <v>398</v>
       </c>
@@ -13287,7 +13288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8">
       <c r="A441">
         <v>399</v>
       </c>
@@ -13307,7 +13308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8">
       <c r="A442">
         <v>400</v>
       </c>
@@ -13327,7 +13328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8">
       <c r="A443">
         <v>401</v>
       </c>
@@ -13347,7 +13348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8">
       <c r="A444">
         <v>402</v>
       </c>
@@ -13367,7 +13368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8">
       <c r="A445">
         <v>403</v>
       </c>
@@ -13387,7 +13388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8">
       <c r="A446">
         <v>404</v>
       </c>
@@ -13407,7 +13408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8">
       <c r="A447">
         <v>405</v>
       </c>
@@ -13429,7 +13430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8">
       <c r="A448">
         <v>406</v>
       </c>
@@ -13451,7 +13452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8">
       <c r="A449">
         <v>407</v>
       </c>
@@ -13473,7 +13474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8">
       <c r="A450">
         <v>408</v>
       </c>
@@ -13495,7 +13496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8">
       <c r="A451">
         <v>409</v>
       </c>
@@ -13517,7 +13518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="452" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:8" ht="16" thickBot="1">
       <c r="A452">
         <v>410</v>
       </c>
@@ -13539,7 +13540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="453" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="453" spans="1:8" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>